<commit_message>
Day 3 Framework update
</commit_message>
<xml_diff>
--- a/data/TC01.xlsx
+++ b/data/TC01.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Mylearning$2</t>
+  </si>
+  <si>
+    <t>zahira@credosystemz.sandbox</t>
+  </si>
+  <si>
+    <t>Waseem@20</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -386,7 +392,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,19 +404,28 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Implementation Report and Selenium Wrapper
</commit_message>
<xml_diff>
--- a/data/TC01.xlsx
+++ b/data/TC01.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
@@ -29,29 +29,15 @@
   <si>
     <t>Mylearning$2</t>
   </si>
-  <si>
-    <t>zahira@credosystemz.sandbox</t>
-  </si>
-  <si>
-    <t>Waseem@20</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,16 +60,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,11 +366,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -411,21 +392,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
CI Integration with Jenkins
</commit_message>
<xml_diff>
--- a/data/TC01.xlsx
+++ b/data/TC01.xlsx
@@ -27,7 +27,7 @@
     <t>mathan@credosystemz.sanbox</t>
   </si>
   <si>
-    <t>Mylearning$2</t>
+    <t>Mylearning$3</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>